<commit_message>
Upado os desafios que estavam no meu HD antigo.
</commit_message>
<xml_diff>
--- a/SpotifyClone-Non-NormalizedTable.xlsx
+++ b/SpotifyClone-Non-NormalizedTable.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="75">
   <si>
     <t xml:space="preserve">usuario_id</t>
   </si>
@@ -157,64 +157,61 @@
     <t xml:space="preserve">álbum</t>
   </si>
   <si>
+    <t xml:space="preserve">name_album</t>
+  </si>
+  <si>
+    <t xml:space="preserve">artist_id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">artists</t>
+  </si>
+  <si>
+    <t xml:space="preserve">plans</t>
+  </si>
+  <si>
     <t xml:space="preserve">name</t>
   </si>
   <si>
-    <t xml:space="preserve">artist_id</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Artists</t>
-  </si>
-  <si>
-    <t xml:space="preserve">plans</t>
-  </si>
-  <si>
     <t xml:space="preserve">plan</t>
   </si>
   <si>
     <t xml:space="preserve">price</t>
   </si>
   <si>
-    <t xml:space="preserve">followed_artists</t>
-  </si>
-  <si>
-    <t xml:space="preserve">followed_ones</t>
+    <t xml:space="preserve">followed</t>
   </si>
   <si>
     <t xml:space="preserve">songs</t>
   </si>
   <si>
+    <t xml:space="preserve">song_id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">name_songs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"Soul For Us"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"Reflections Of Magic"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"Dance With Her Own"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"Troubles Of My Inner Fire"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"Time Fireworks"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"Magic Circus"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"Honey, So Do I"</t>
+  </si>
+  <si>
     <t xml:space="preserve">reproduction_history</t>
-  </si>
-  <si>
-    <t xml:space="preserve">song_id</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rep_id</t>
-  </si>
-  <si>
-    <t xml:space="preserve">history</t>
-  </si>
-  <si>
-    <t xml:space="preserve">"Soul For Us"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">"Reflections Of Magic"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">"Dance With Her Own"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">"Troubles Of My Inner Fire"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">"Time Fireworks"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">"Magic Circus"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">"Honey, So Do I"</t>
   </si>
   <si>
     <t xml:space="preserve">"Sweetie, Let's Go Wild"</t>
@@ -258,11 +255,12 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -278,6 +276,13 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -334,7 +339,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -383,8 +388,12 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -406,8 +415,8 @@
   </sheetPr>
   <dimension ref="A1:I1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A25" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F34" activeCellId="0" sqref="F34"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D44" activeCellId="0" sqref="D44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8515625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -834,17 +843,17 @@
         <v>46</v>
       </c>
       <c r="B25" s="10" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="C25" s="10"/>
       <c r="E25" s="10" t="s">
         <v>43</v>
       </c>
       <c r="F25" s="10" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="G25" s="10" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -910,64 +919,110 @@
       <c r="B30" s="6"/>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F32" s="10" t="s">
-        <v>51</v>
+      <c r="F32" s="10"/>
+      <c r="H32" s="12" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="E33" s="10" t="s">
+      <c r="E33" s="10"/>
+      <c r="F33" s="0"/>
+      <c r="G33" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="F33" s="10" t="s">
-        <v>52</v>
+      <c r="H33" s="10" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="E34" s="8" t="n">
-        <v>1</v>
-      </c>
-      <c r="F34" s="7" t="s">
-        <v>10</v>
+      <c r="E34" s="0"/>
+      <c r="F34" s="0"/>
+      <c r="G34" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="H34" s="11" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="E35" s="8" t="n">
-        <v>2</v>
-      </c>
-      <c r="F35" s="7" t="s">
-        <v>14</v>
+      <c r="E35" s="0"/>
+      <c r="F35" s="0"/>
+      <c r="G35" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="H35" s="11" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="E36" s="8" t="n">
-        <v>3</v>
-      </c>
-      <c r="F36" s="7" t="s">
-        <v>18</v>
+      <c r="E36" s="0"/>
+      <c r="F36" s="0"/>
+      <c r="G36" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="H36" s="11" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="E37" s="8" t="n">
-        <v>4</v>
-      </c>
-      <c r="F37" s="7" t="s">
-        <v>21</v>
+      <c r="E37" s="0"/>
+      <c r="F37" s="0"/>
+      <c r="G37" s="11" t="n">
+        <v>2</v>
+      </c>
+      <c r="H37" s="11" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F38" s="11"/>
+      <c r="G38" s="11" t="n">
+        <v>2</v>
+      </c>
+      <c r="H38" s="11" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F39" s="11"/>
+      <c r="G39" s="11" t="n">
+        <v>3</v>
+      </c>
+      <c r="H39" s="11" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G40" s="11" t="n">
+        <v>3</v>
+      </c>
+      <c r="H40" s="11" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G41" s="11" t="n">
+        <v>4</v>
+      </c>
+      <c r="H41" s="11" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B42" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="F42" s="10" t="s">
-        <v>54</v>
-      </c>
+      <c r="E42" s="0"/>
+      <c r="F42" s="0"/>
+      <c r="G42" s="0"/>
+      <c r="H42" s="0"/>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A43" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="B43" s="10" t="s">
         <v>55</v>
-      </c>
-      <c r="B43" s="10" t="s">
-        <v>45</v>
       </c>
       <c r="C43" s="10" t="s">
         <v>22</v>
@@ -975,19 +1030,17 @@
       <c r="D43" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="E43" s="10" t="s">
-        <v>56</v>
-      </c>
-      <c r="F43" s="12" t="s">
-        <v>57</v>
-      </c>
+      <c r="E43" s="0"/>
+      <c r="F43" s="0"/>
+      <c r="G43" s="0"/>
+      <c r="H43" s="0"/>
     </row>
     <row r="44" customFormat="false" ht="32.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A44" s="11" t="n">
         <v>1</v>
       </c>
       <c r="B44" s="11" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C44" s="11" t="n">
         <v>1</v>
@@ -995,19 +1048,17 @@
       <c r="D44" s="11" t="n">
         <v>1</v>
       </c>
-      <c r="E44" s="11" t="n">
-        <v>1</v>
-      </c>
-      <c r="F44" s="7" t="s">
-        <v>9</v>
-      </c>
+      <c r="E44" s="0"/>
+      <c r="F44" s="0"/>
+      <c r="G44" s="0"/>
+      <c r="H44" s="0"/>
     </row>
     <row r="45" customFormat="false" ht="35.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A45" s="11" t="n">
         <v>2</v>
       </c>
       <c r="B45" s="11" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C45" s="11" t="n">
         <v>1</v>
@@ -1015,19 +1066,17 @@
       <c r="D45" s="11" t="n">
         <v>1</v>
       </c>
-      <c r="E45" s="11" t="n">
-        <v>2</v>
-      </c>
-      <c r="F45" s="7" t="s">
-        <v>13</v>
-      </c>
+      <c r="E45" s="0"/>
+      <c r="F45" s="0"/>
+      <c r="G45" s="0"/>
+      <c r="H45" s="0"/>
     </row>
     <row r="46" customFormat="false" ht="44" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A46" s="11" t="n">
         <v>3</v>
       </c>
       <c r="B46" s="11" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C46" s="11" t="n">
         <v>1</v>
@@ -1035,19 +1084,17 @@
       <c r="D46" s="11" t="n">
         <v>1</v>
       </c>
-      <c r="E46" s="11" t="n">
-        <v>3</v>
-      </c>
-      <c r="F46" s="7" t="s">
-        <v>17</v>
-      </c>
+      <c r="E46" s="0"/>
+      <c r="F46" s="0"/>
+      <c r="G46" s="0"/>
+      <c r="H46" s="0"/>
     </row>
     <row r="47" customFormat="false" ht="38.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A47" s="11" t="n">
         <v>4</v>
       </c>
       <c r="B47" s="11" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C47" s="11" t="n">
         <v>2</v>
@@ -1055,19 +1102,17 @@
       <c r="D47" s="11" t="n">
         <v>1</v>
       </c>
-      <c r="E47" s="11" t="n">
-        <v>4</v>
-      </c>
-      <c r="F47" s="1" t="s">
-        <v>20</v>
-      </c>
+      <c r="E47" s="0"/>
+      <c r="F47" s="0"/>
+      <c r="G47" s="0"/>
+      <c r="H47" s="0"/>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A48" s="11" t="n">
         <v>5</v>
       </c>
       <c r="B48" s="11" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C48" s="11" t="n">
         <v>2</v>
@@ -1081,7 +1126,7 @@
         <v>6</v>
       </c>
       <c r="B49" s="11" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C49" s="11" t="n">
         <v>3</v>
@@ -1095,7 +1140,7 @@
         <v>7</v>
       </c>
       <c r="B50" s="11" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C50" s="11" t="n">
         <v>3</v>
@@ -1103,19 +1148,29 @@
       <c r="D50" s="11" t="n">
         <v>2</v>
       </c>
+      <c r="F50" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="G50" s="10"/>
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A51" s="11" t="n">
         <v>8</v>
       </c>
       <c r="B51" s="11" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C51" s="11" t="n">
         <v>3</v>
       </c>
       <c r="D51" s="11" t="n">
         <v>2</v>
+      </c>
+      <c r="E51" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="F51" s="13" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1123,13 +1178,19 @@
         <v>9</v>
       </c>
       <c r="B52" s="11" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C52" s="11" t="n">
         <v>3</v>
       </c>
       <c r="D52" s="11" t="n">
         <v>2</v>
+      </c>
+      <c r="E52" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="F52" s="11" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1137,13 +1198,19 @@
         <v>10</v>
       </c>
       <c r="B53" s="11" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C53" s="11" t="n">
         <v>4</v>
       </c>
       <c r="D53" s="11" t="n">
         <v>3</v>
+      </c>
+      <c r="E53" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="F53" s="11" t="n">
+        <v>6</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1151,13 +1218,19 @@
         <v>11</v>
       </c>
       <c r="B54" s="11" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C54" s="11" t="n">
         <v>4</v>
       </c>
       <c r="D54" s="11" t="n">
         <v>3</v>
+      </c>
+      <c r="E54" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="F54" s="11" t="n">
+        <v>14</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1165,13 +1238,19 @@
         <v>12</v>
       </c>
       <c r="B55" s="11" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C55" s="11" t="n">
         <v>4</v>
       </c>
       <c r="D55" s="11" t="n">
         <v>3</v>
+      </c>
+      <c r="E55" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="F55" s="11" t="n">
+        <v>16</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1179,13 +1258,19 @@
         <v>13</v>
       </c>
       <c r="B56" s="11" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C56" s="11" t="n">
         <v>4</v>
       </c>
       <c r="D56" s="11" t="n">
         <v>3</v>
+      </c>
+      <c r="E56" s="11" t="n">
+        <v>2</v>
+      </c>
+      <c r="F56" s="11" t="n">
+        <v>13</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1193,13 +1278,19 @@
         <v>14</v>
       </c>
       <c r="B57" s="11" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C57" s="11" t="n">
         <v>4</v>
       </c>
       <c r="D57" s="11" t="n">
         <v>3</v>
+      </c>
+      <c r="E57" s="11" t="n">
+        <v>2</v>
+      </c>
+      <c r="F57" s="11" t="n">
+        <v>17</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1207,13 +1298,19 @@
         <v>15</v>
       </c>
       <c r="B58" s="11" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C58" s="11" t="n">
         <v>4</v>
       </c>
       <c r="D58" s="11" t="n">
         <v>3</v>
+      </c>
+      <c r="E58" s="11" t="n">
+        <v>2</v>
+      </c>
+      <c r="F58" s="11" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1221,13 +1318,19 @@
         <v>16</v>
       </c>
       <c r="B59" s="11" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C59" s="11" t="n">
         <v>5</v>
       </c>
       <c r="D59" s="11" t="n">
         <v>4</v>
+      </c>
+      <c r="E59" s="11" t="n">
+        <v>2</v>
+      </c>
+      <c r="F59" s="11" t="n">
+        <v>15</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1235,12 +1338,18 @@
         <v>17</v>
       </c>
       <c r="B60" s="11" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C60" s="11" t="n">
         <v>5</v>
       </c>
       <c r="D60" s="11" t="n">
+        <v>4</v>
+      </c>
+      <c r="E60" s="11" t="n">
+        <v>3</v>
+      </c>
+      <c r="F60" s="11" t="n">
         <v>4</v>
       </c>
     </row>
@@ -1249,13 +1358,19 @@
         <v>18</v>
       </c>
       <c r="B61" s="11" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C61" s="11" t="n">
         <v>5</v>
       </c>
       <c r="D61" s="11" t="n">
         <v>4</v>
+      </c>
+      <c r="E61" s="11" t="n">
+        <v>3</v>
+      </c>
+      <c r="F61" s="11" t="n">
+        <v>16</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1263,66 +1378,185 @@
       <c r="B62" s="11"/>
       <c r="C62" s="11"/>
       <c r="D62" s="11"/>
+      <c r="E62" s="11" t="n">
+        <v>3</v>
+      </c>
+      <c r="F62" s="11" t="n">
+        <v>6</v>
+      </c>
     </row>
     <row r="63" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A63" s="11"/>
       <c r="B63" s="11"/>
       <c r="C63" s="11"/>
       <c r="D63" s="11"/>
+      <c r="E63" s="11" t="n">
+        <v>4</v>
+      </c>
+      <c r="F63" s="11" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="64" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A64" s="11"/>
       <c r="B64" s="11"/>
       <c r="C64" s="11"/>
       <c r="D64" s="11"/>
+      <c r="E64" s="11" t="n">
+        <v>4</v>
+      </c>
+      <c r="F64" s="11" t="n">
+        <v>18</v>
+      </c>
     </row>
     <row r="65" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A65" s="11"/>
       <c r="B65" s="11"/>
       <c r="C65" s="11"/>
       <c r="D65" s="11"/>
+      <c r="E65" s="11" t="n">
+        <v>4</v>
+      </c>
+      <c r="F65" s="11" t="n">
+        <v>11</v>
+      </c>
     </row>
     <row r="66" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A66" s="11"/>
       <c r="B66" s="11"/>
       <c r="C66" s="11"/>
       <c r="D66" s="11"/>
+      <c r="E66" s="11"/>
+      <c r="F66" s="11"/>
     </row>
     <row r="67" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A67" s="11"/>
       <c r="B67" s="11"/>
       <c r="C67" s="11"/>
       <c r="D67" s="11"/>
+      <c r="E67" s="11"/>
+      <c r="F67" s="11"/>
     </row>
     <row r="68" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A68" s="11"/>
       <c r="B68" s="11"/>
       <c r="C68" s="11"/>
       <c r="D68" s="11"/>
+      <c r="E68" s="11"/>
+      <c r="F68" s="11"/>
     </row>
     <row r="69" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A69" s="11"/>
       <c r="B69" s="11"/>
       <c r="C69" s="11"/>
       <c r="D69" s="11"/>
+      <c r="E69" s="11"/>
+      <c r="F69" s="11"/>
     </row>
     <row r="70" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A70" s="11"/>
       <c r="B70" s="11"/>
       <c r="C70" s="11"/>
       <c r="D70" s="11"/>
+      <c r="E70" s="11"/>
+      <c r="F70" s="11"/>
     </row>
     <row r="71" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A71" s="11"/>
       <c r="B71" s="11"/>
       <c r="C71" s="11"/>
       <c r="D71" s="11"/>
+      <c r="E71" s="11"/>
+      <c r="F71" s="11"/>
     </row>
     <row r="72" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A72" s="11"/>
       <c r="B72" s="11"/>
       <c r="C72" s="11"/>
       <c r="D72" s="11"/>
+      <c r="E72" s="11"/>
+      <c r="F72" s="11"/>
+    </row>
+    <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E73" s="11"/>
+      <c r="F73" s="11"/>
+    </row>
+    <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E74" s="11"/>
+      <c r="F74" s="11"/>
+    </row>
+    <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E75" s="11"/>
+      <c r="F75" s="11"/>
+    </row>
+    <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E76" s="11"/>
+      <c r="F76" s="11"/>
+    </row>
+    <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E77" s="11"/>
+      <c r="F77" s="11"/>
+    </row>
+    <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E78" s="11"/>
+      <c r="F78" s="11"/>
+    </row>
+    <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E79" s="11"/>
+      <c r="F79" s="11"/>
+    </row>
+    <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E80" s="11"/>
+      <c r="F80" s="11"/>
+    </row>
+    <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E81" s="11"/>
+      <c r="F81" s="11"/>
+    </row>
+    <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E82" s="11"/>
+      <c r="F82" s="11"/>
+    </row>
+    <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E83" s="11"/>
+      <c r="F83" s="11"/>
+    </row>
+    <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E84" s="11"/>
+      <c r="F84" s="11"/>
+    </row>
+    <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F85" s="11"/>
+    </row>
+    <row r="86" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F86" s="11"/>
+    </row>
+    <row r="87" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F87" s="11"/>
+    </row>
+    <row r="88" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F88" s="11"/>
+    </row>
+    <row r="89" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F89" s="11"/>
+    </row>
+    <row r="90" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F90" s="11"/>
+    </row>
+    <row r="91" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F91" s="11"/>
+    </row>
+    <row r="92" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F92" s="11"/>
+    </row>
+    <row r="93" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F93" s="11"/>
+    </row>
+    <row r="94" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F94" s="11"/>
+    </row>
+    <row r="95" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F95" s="11"/>
     </row>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>

</xml_diff>